<commit_message>
magius product type and product code
</commit_message>
<xml_diff>
--- a/magius/checklist.xlsx
+++ b/magius/checklist.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/magius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E8516-A69F-DF46-A311-347DC6429502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11403170-EF84-9A43-9E9A-64A65563F609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{EC86A737-DBCB-9E4E-9736-CFEB633AEAE9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{EC86A737-DBCB-9E4E-9736-CFEB633AEAE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="118">
   <si>
     <t>year</t>
   </si>
@@ -312,6 +312,81 @@
   </si>
   <si>
     <t>Neighborhood Defense Corps RPG</t>
+  </si>
+  <si>
+    <t>product_type</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>13-1</t>
+  </si>
+  <si>
+    <t>rulebook</t>
+  </si>
+  <si>
+    <t>13-3</t>
+  </si>
+  <si>
+    <t>13-4</t>
+  </si>
+  <si>
+    <t>13-13</t>
+  </si>
+  <si>
+    <t>13-15</t>
+  </si>
+  <si>
+    <t>13-8</t>
+  </si>
+  <si>
+    <t>13-17</t>
+  </si>
+  <si>
+    <t>13-22</t>
+  </si>
+  <si>
+    <t>13-14</t>
+  </si>
+  <si>
+    <t>13-5</t>
+  </si>
+  <si>
+    <t>13-16</t>
+  </si>
+  <si>
+    <t>13-11</t>
+  </si>
+  <si>
+    <t>13-2</t>
+  </si>
+  <si>
+    <t>13-10</t>
+  </si>
+  <si>
+    <t>13-9</t>
+  </si>
+  <si>
+    <t>13-6</t>
+  </si>
+  <si>
+    <t>13-7</t>
+  </si>
+  <si>
+    <t>13-12</t>
+  </si>
+  <si>
+    <t>13-24</t>
+  </si>
+  <si>
+    <t>13-28</t>
+  </si>
+  <si>
+    <t>13-23</t>
+  </si>
+  <si>
+    <t>supplement</t>
   </si>
 </sst>
 </file>
@@ -672,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E4EB47-E4AF-944A-9098-51681AF52635}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F3" sqref="F3:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,9 +760,10 @@
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,8 +779,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1995</v>
       </c>
@@ -720,8 +802,14 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1995</v>
       </c>
@@ -737,8 +825,14 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -754,8 +848,14 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1995</v>
       </c>
@@ -771,8 +871,14 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1995</v>
       </c>
@@ -788,8 +894,14 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -805,8 +917,14 @@
       <c r="E7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -822,8 +940,14 @@
       <c r="E8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1995</v>
       </c>
@@ -839,8 +963,14 @@
       <c r="E9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1995</v>
       </c>
@@ -856,8 +986,14 @@
       <c r="E10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1995</v>
       </c>
@@ -873,8 +1009,14 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1995</v>
       </c>
@@ -890,8 +1032,14 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1996</v>
       </c>
@@ -907,8 +1055,14 @@
       <c r="E13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1996</v>
       </c>
@@ -924,8 +1078,14 @@
       <c r="E14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1996</v>
       </c>
@@ -941,8 +1101,14 @@
       <c r="E15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1996</v>
       </c>
@@ -958,8 +1124,14 @@
       <c r="E16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1996</v>
       </c>
@@ -975,8 +1147,14 @@
       <c r="E17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1996</v>
       </c>
@@ -992,8 +1170,14 @@
       <c r="E18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1997</v>
       </c>
@@ -1009,8 +1193,11 @@
       <c r="E19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1997</v>
       </c>
@@ -1026,8 +1213,14 @@
       <c r="E20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1997</v>
       </c>
@@ -1043,8 +1236,11 @@
       <c r="E21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1997</v>
       </c>
@@ -1060,8 +1256,11 @@
       <c r="E22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1997</v>
       </c>
@@ -1077,8 +1276,11 @@
       <c r="E23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1997</v>
       </c>
@@ -1094,8 +1296,14 @@
       <c r="E24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1997</v>
       </c>
@@ -1111,8 +1319,11 @@
       <c r="E25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1997</v>
       </c>
@@ -1128,8 +1339,11 @@
       <c r="E26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1997</v>
       </c>
@@ -1145,8 +1359,14 @@
       <c r="E27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1998</v>
       </c>
@@ -1162,8 +1382,14 @@
       <c r="E28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1998</v>
       </c>
@@ -1179,8 +1405,11 @@
       <c r="E29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -1195,6 +1424,9 @@
       </c>
       <c r="E30" t="s">
         <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>